<commit_message>
Pruebas de funcionalidad global completadas
</commit_message>
<xml_diff>
--- a/data/examples/resultados_informe_politica_demo_test.xlsx
+++ b/data/examples/resultados_informe_politica_demo_test.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,37 +518,87 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>scale_min</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>scale_max</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>tipo_informe</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>model_name</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>pipeline_version</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>run_id</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>metadata.skipped</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>metadata.skip_reason</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>metadata.segmenter_status</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.pipeline_version</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.pipeline_version_history</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.run_id</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.run_id_history</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.criteria_version</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>metadata.criteria_versions</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>dimension_id</t>
         </is>
       </c>
     </row>
@@ -617,37 +667,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U2" t="b">
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X2" t="b">
         <v>1</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Resumen Ejecutivo</t>
         </is>
       </c>
     </row>
@@ -716,37 +808,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U3" t="b">
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Resumen Ejecutivo</t>
         </is>
       </c>
     </row>
@@ -815,37 +949,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U4" t="b">
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X4" t="b">
         <v>1</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Descripción de la política nacional</t>
         </is>
       </c>
     </row>
@@ -914,37 +1090,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U5" t="b">
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X5" t="b">
         <v>1</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>Descripción de la política nacional</t>
         </is>
       </c>
     </row>
@@ -1013,37 +1231,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U6" t="b">
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X6" t="b">
         <v>1</v>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="Y6" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Análisis de los resultados de la política nacional</t>
         </is>
       </c>
     </row>
@@ -1112,37 +1372,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U7" t="b">
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X7" t="b">
         <v>1</v>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
+      <c r="Z7" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>Análisis de los resultados de la política nacional</t>
         </is>
       </c>
     </row>
@@ -1211,37 +1513,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U8" t="b">
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X8" t="b">
         <v>1</v>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
+      <c r="Z8" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>Análisis de los resultados de la política nacional</t>
         </is>
       </c>
     </row>
@@ -1310,37 +1654,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U9" t="b">
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X9" t="b">
         <v>1</v>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="Y9" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
+      <c r="Z9" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>Análisis de los resultados de la política nacional</t>
         </is>
       </c>
     </row>
@@ -1409,37 +1795,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U10" t="b">
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X10" t="b">
         <v>1</v>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="Y10" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="Z10" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -1508,37 +1936,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U11" t="b">
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X11" t="b">
         <v>1</v>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="Z11" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -1607,37 +2077,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U12" t="b">
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X12" t="b">
         <v>1</v>
       </c>
-      <c r="V12" t="inlineStr">
+      <c r="Y12" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr">
+      <c r="Z12" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -1706,37 +2218,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U13" t="b">
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X13" t="b">
         <v>1</v>
       </c>
-      <c r="V13" t="inlineStr">
+      <c r="Y13" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr">
+      <c r="Z13" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -1805,37 +2359,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U14" t="b">
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X14" t="b">
         <v>1</v>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="Y14" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
+      <c r="Z14" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -1904,37 +2500,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U15" t="b">
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X15" t="b">
         <v>1</v>
       </c>
-      <c r="V15" t="inlineStr">
+      <c r="Y15" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W15" t="inlineStr">
+      <c r="Z15" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>Análisis de la implementación</t>
         </is>
       </c>
     </row>
@@ -2003,37 +2641,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U16" t="b">
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X16" t="b">
         <v>1</v>
       </c>
-      <c r="V16" t="inlineStr">
+      <c r="Y16" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W16" t="inlineStr">
+      <c r="Z16" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>Conclusiones</t>
         </is>
       </c>
     </row>
@@ -2102,37 +2782,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U17" t="b">
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X17" t="b">
         <v>1</v>
       </c>
-      <c r="V17" t="inlineStr">
+      <c r="Y17" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W17" t="inlineStr">
+      <c r="Z17" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>Recomendaciones</t>
         </is>
       </c>
     </row>
@@ -2201,37 +2923,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="T18" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U18" t="b">
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X18" t="b">
         <v>1</v>
       </c>
-      <c r="V18" t="inlineStr">
+      <c r="Y18" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W18" t="inlineStr">
+      <c r="Z18" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>Recomendaciones</t>
         </is>
       </c>
     </row>
@@ -2300,37 +3064,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U19" t="b">
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X19" t="b">
         <v>1</v>
       </c>
-      <c r="V19" t="inlineStr">
+      <c r="Y19" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W19" t="inlineStr">
+      <c r="Z19" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>Anexos</t>
         </is>
       </c>
     </row>
@@ -2399,37 +3205,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U20" t="b">
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X20" t="b">
         <v>1</v>
       </c>
-      <c r="V20" t="inlineStr">
+      <c r="Y20" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W20" t="inlineStr">
+      <c r="Z20" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>Anexos</t>
         </is>
       </c>
     </row>
@@ -2494,37 +3342,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
+      <c r="T21" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U21" t="b">
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X21" t="b">
         <v>1</v>
       </c>
-      <c r="V21" t="inlineStr">
+      <c r="Y21" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W21" t="inlineStr">
+      <c r="Z21" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>Preguntas complementarias</t>
         </is>
       </c>
     </row>
@@ -2589,37 +3479,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U22" t="b">
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X22" t="b">
         <v>1</v>
       </c>
-      <c r="V22" t="inlineStr">
+      <c r="Y22" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W22" t="inlineStr">
+      <c r="Z22" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>Preguntas complementarias</t>
         </is>
       </c>
     </row>
@@ -2684,37 +3616,79 @@
           <t>2024.1</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>2025-10-26T11:29:42.909132</t>
-        </is>
-      </c>
-      <c r="U23" t="b">
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>2025-10-26T22:25:27.187688</t>
+        </is>
+      </c>
+      <c r="X23" t="b">
         <v>1</v>
       </c>
-      <c r="V23" t="inlineStr">
+      <c r="Y23" t="inlineStr">
         <is>
           <t>missing_section</t>
         </is>
       </c>
-      <c r="W23" t="inlineStr">
+      <c r="Z23" t="inlineStr">
         <is>
           <t>missing</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>["0.1.0"]</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>["a1de0ddd622744788ce686c90a8f7dbb"]</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>["2024.1"]</t>
+        </is>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>Preguntas complementarias</t>
         </is>
       </c>
     </row>
@@ -2729,7 +3703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2768,6 +3742,16 @@
           <t>normalized_score</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>raw_score</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>criteria_version</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2794,6 +3778,14 @@
       <c r="F2" t="n">
         <v>0</v>
       </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2820,6 +3812,14 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2846,6 +3846,14 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2872,6 +3880,14 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2898,6 +3914,14 @@
       <c r="F6" t="n">
         <v>0</v>
       </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2924,6 +3948,14 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2949,6 +3981,14 @@
       </c>
       <c r="F8" t="n">
         <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -2971,6 +4011,14 @@
       </c>
       <c r="F9" t="n">
         <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024.1</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2984,7 +4032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3025,54 +4073,54 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>criteria_version</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>segmenter_flagged_breakdown</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>segmenter_flagged_sections</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>missing_sections</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>empty_sections</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>segmenter_warning</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>run_id</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>model_name</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>tipo_informe</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>pipeline_version</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>criteria_version</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>timestamp</t>
@@ -3096,6 +4144,11 @@
       <c r="U1" s="1" t="inlineStr">
         <is>
           <t>extra_pipeline_version</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>extra_criteria_hash</t>
         </is>
       </c>
     </row>
@@ -3120,60 +4173,60 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>2024.1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>{'missing': 8, 'empty': 0, 'found': 0}</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>8</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>['resumen_ejecutivo', 'descripcion_politica', 'analisis_resultados', 'analisis_implementacion', 'conclusiones', 'recomendaciones', 'anexos', 'Preguntas complementarias']</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Se detectaron secciones ausentes o sin contenido durante la evaluación.</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>f8e202da056c46b48a6e0608d49a82d5</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>a1de0ddd622744788ce686c90a8f7dbb</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>gpt-4o-mini</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>politica_nacional</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>0.1.0</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2024.1</t>
+          <t>0.1.0</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-10-26T11:29:42.909132</t>
+          <t>2025-10-26T22:25:27.187688</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{'model_name': 'gpt-4o-mini', 'retries': 2, 'backoff_factor': 2.0, 'timeout_seconds': 60.0, 'prompt_batch_size': 1, 'log_level': 'INFO', 'log_file': None, 'ai_provider': 'mock', 'run_id': 'f8e202da056c46b48a6e0608d49a82d5', 'document_id': None, 'extra_instructions': None, 'splitter_log_level': 'info', 'splitter_normalize_newlines': True}</t>
+          <t>{'model_name': 'gpt-4o-mini', 'retries': 2, 'backoff_factor': 2.0, 'timeout_seconds': 60.0, 'prompt_batch_size': 1, 'log_level': 'INFO', 'log_file': None, 'ai_provider': 'mock', 'run_id': 'a1de0ddd622744788ce686c90a8f7dbb', 'document_id': None, 'extra_instructions': None, 'splitter_log_level': 'info', 'splitter_normalize_newlines': True}</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -3189,6 +4242,11 @@
       <c r="U2" t="inlineStr">
         <is>
           <t>0.1.0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>5c7fdfed71a0c2f52a7171577c792d9c236420ba3b160ba8e2305c65aa06bc0c</t>
         </is>
       </c>
     </row>

</xml_diff>